<commit_message>
Updates to restaurant data and scripts
</commit_message>
<xml_diff>
--- a/Toast/Wine Product IDs.xlsx
+++ b/Toast/Wine Product IDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\projects\old-bar-pi\Toast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A469CF6-17A6-48EB-8F71-108A0977773C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81072711-0CF7-4F1E-8FBF-8A930B4BB2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="2320" windowWidth="18210" windowHeight="15280" xr2:uid="{3FEA0871-F7CF-48E3-9576-476D9F68DB94}"/>
+    <workbookView xWindow="23010" yWindow="2850" windowWidth="14640" windowHeight="15280" xr2:uid="{3FEA0871-F7CF-48E3-9576-476D9F68DB94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -615,15 +615,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F81134EC-7B5E-49C7-82CD-86216D921A1F}">
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32.26953125" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -631,17 +631,17 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>126674376</v>
       </c>
     </row>
@@ -649,7 +649,7 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>126654733</v>
       </c>
     </row>
@@ -657,7 +657,7 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>126577844</v>
       </c>
     </row>
@@ -666,10 +666,10 @@
         <v>6</v>
       </c>
       <c r="B5">
+        <v>126717776</v>
+      </c>
+      <c r="C5">
         <v>126675701</v>
-      </c>
-      <c r="C5">
-        <v>126717776</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -677,10 +677,10 @@
         <v>7</v>
       </c>
       <c r="B6">
+        <v>108923090</v>
+      </c>
+      <c r="C6">
         <v>126662461</v>
-      </c>
-      <c r="C6">
-        <v>108923090</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -688,17 +688,17 @@
         <v>8</v>
       </c>
       <c r="B7">
+        <v>126700375</v>
+      </c>
+      <c r="C7">
         <v>86838560</v>
-      </c>
-      <c r="C7">
-        <v>126700375</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>126665706</v>
       </c>
     </row>
@@ -707,17 +707,17 @@
         <v>10</v>
       </c>
       <c r="B9">
+        <v>226472787</v>
+      </c>
+      <c r="C9">
         <v>226396480</v>
-      </c>
-      <c r="C9">
-        <v>226472787</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>126652489</v>
       </c>
     </row>
@@ -726,10 +726,10 @@
         <v>12</v>
       </c>
       <c r="B11">
+        <v>126707734</v>
+      </c>
+      <c r="C11">
         <v>126666591</v>
-      </c>
-      <c r="C11">
-        <v>126707734</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -737,10 +737,10 @@
         <v>13</v>
       </c>
       <c r="B12">
+        <v>138978515</v>
+      </c>
+      <c r="C12">
         <v>139085317</v>
-      </c>
-      <c r="C12">
-        <v>138978515</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -748,10 +748,10 @@
         <v>14</v>
       </c>
       <c r="B13">
+        <v>134751298</v>
+      </c>
+      <c r="C13">
         <v>134727097</v>
-      </c>
-      <c r="C13">
-        <v>134751298</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -759,17 +759,17 @@
         <v>15</v>
       </c>
       <c r="B14">
+        <v>1276497518</v>
+      </c>
+      <c r="C14">
         <v>1276474213</v>
-      </c>
-      <c r="C14">
-        <v>1276497518</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>126653764</v>
       </c>
     </row>
@@ -778,10 +778,10 @@
         <v>17</v>
       </c>
       <c r="B16">
+        <v>126701381</v>
+      </c>
+      <c r="C16">
         <v>126657095</v>
-      </c>
-      <c r="C16">
-        <v>126701381</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -789,10 +789,10 @@
         <v>18</v>
       </c>
       <c r="B17">
+        <v>126713038</v>
+      </c>
+      <c r="C17">
         <v>126586184</v>
-      </c>
-      <c r="C17">
-        <v>126713038</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -800,17 +800,17 @@
         <v>19</v>
       </c>
       <c r="B18">
+        <v>126697904</v>
+      </c>
+      <c r="C18">
         <v>126655512</v>
-      </c>
-      <c r="C18">
-        <v>126697904</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>134692033</v>
       </c>
     </row>
@@ -819,17 +819,17 @@
         <v>21</v>
       </c>
       <c r="B20">
+        <v>126710903</v>
+      </c>
+      <c r="C20">
         <v>126668956</v>
-      </c>
-      <c r="C20">
-        <v>126710903</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>126658957</v>
       </c>
     </row>
@@ -838,10 +838,10 @@
         <v>23</v>
       </c>
       <c r="B22">
+        <v>226476258</v>
+      </c>
+      <c r="C22">
         <v>226401294</v>
-      </c>
-      <c r="C22">
-        <v>226476258</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -849,10 +849,10 @@
         <v>24</v>
       </c>
       <c r="B23">
+        <v>134741583</v>
+      </c>
+      <c r="C23">
         <v>134684785</v>
-      </c>
-      <c r="C23">
-        <v>134741583</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -860,17 +860,17 @@
         <v>25</v>
       </c>
       <c r="B24">
+        <v>126695589</v>
+      </c>
+      <c r="C24">
         <v>126582598</v>
-      </c>
-      <c r="C24">
-        <v>126695589</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>134690352</v>
       </c>
     </row>
@@ -879,10 +879,10 @@
         <v>27</v>
       </c>
       <c r="B26">
+        <v>126702220</v>
+      </c>
+      <c r="C26">
         <v>126588031</v>
-      </c>
-      <c r="C26">
-        <v>126702220</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -890,17 +890,17 @@
         <v>28</v>
       </c>
       <c r="B27">
+        <v>108923080</v>
+      </c>
+      <c r="C27">
         <v>126600823</v>
-      </c>
-      <c r="C27">
-        <v>108923080</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>86790527</v>
       </c>
     </row>
@@ -908,7 +908,7 @@
       <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>1918727844</v>
       </c>
     </row>
@@ -916,7 +916,7 @@
       <c r="A30" t="s">
         <v>31</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>126619457</v>
       </c>
     </row>
@@ -925,10 +925,10 @@
         <v>32</v>
       </c>
       <c r="B31">
+        <v>1394304966</v>
+      </c>
+      <c r="C31">
         <v>1394368994</v>
-      </c>
-      <c r="C31">
-        <v>1394304966</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -936,10 +936,10 @@
         <v>33</v>
       </c>
       <c r="B32">
+        <v>126698677</v>
+      </c>
+      <c r="C32">
         <v>126616181</v>
-      </c>
-      <c r="C32">
-        <v>126698677</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -947,10 +947,10 @@
         <v>34</v>
       </c>
       <c r="B33">
+        <v>108923074</v>
+      </c>
+      <c r="C33">
         <v>126617293</v>
-      </c>
-      <c r="C33">
-        <v>108923074</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -958,17 +958,17 @@
         <v>35</v>
       </c>
       <c r="B34">
+        <v>1248969120</v>
+      </c>
+      <c r="C34">
         <v>1248983785</v>
-      </c>
-      <c r="C34">
-        <v>1248969120</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>36</v>
       </c>
-      <c r="B35">
+      <c r="C35">
         <v>126638299</v>
       </c>
     </row>
@@ -977,10 +977,10 @@
         <v>37</v>
       </c>
       <c r="B36">
+        <v>108923076</v>
+      </c>
+      <c r="C36">
         <v>126631693</v>
-      </c>
-      <c r="C36">
-        <v>108923076</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -988,17 +988,17 @@
         <v>39</v>
       </c>
       <c r="B37">
+        <v>126709461</v>
+      </c>
+      <c r="C37">
         <v>126624713</v>
-      </c>
-      <c r="C37">
-        <v>126709461</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>38</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>126630355</v>
       </c>
     </row>
@@ -1006,7 +1006,7 @@
       <c r="A39" t="s">
         <v>40</v>
       </c>
-      <c r="C39">
+      <c r="B39">
         <v>126711696</v>
       </c>
     </row>
@@ -1014,7 +1014,7 @@
       <c r="A40" t="s">
         <v>41</v>
       </c>
-      <c r="C40">
+      <c r="B40">
         <v>362756896</v>
       </c>
     </row>
@@ -1022,7 +1022,7 @@
       <c r="A41" t="s">
         <v>42</v>
       </c>
-      <c r="C41">
+      <c r="B41">
         <v>108923092</v>
       </c>
     </row>
@@ -1031,17 +1031,17 @@
         <v>43</v>
       </c>
       <c r="B43">
+        <v>134743983</v>
+      </c>
+      <c r="C43">
         <v>134708305</v>
-      </c>
-      <c r="C43">
-        <v>134743983</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>46</v>
       </c>
-      <c r="B44">
+      <c r="C44">
         <v>134733882</v>
       </c>
     </row>
@@ -1050,10 +1050,10 @@
         <v>47</v>
       </c>
       <c r="B45">
+        <v>108929178</v>
+      </c>
+      <c r="C45">
         <v>86287019</v>
-      </c>
-      <c r="C45">
-        <v>108929178</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -1061,10 +1061,10 @@
         <v>44</v>
       </c>
       <c r="B46">
+        <v>249833652</v>
+      </c>
+      <c r="C46">
         <v>86292316</v>
-      </c>
-      <c r="C46">
-        <v>249833652</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -1072,10 +1072,10 @@
         <v>45</v>
       </c>
       <c r="B47">
+        <v>362783919</v>
+      </c>
+      <c r="C47">
         <v>362775125</v>
-      </c>
-      <c r="C47">
-        <v>362783919</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -1083,10 +1083,10 @@
         <v>48</v>
       </c>
       <c r="B48">
+        <v>126744935</v>
+      </c>
+      <c r="C48">
         <v>131394447</v>
-      </c>
-      <c r="C48">
-        <v>126744935</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1094,10 +1094,10 @@
         <v>49</v>
       </c>
       <c r="B49">
+        <v>108929180</v>
+      </c>
+      <c r="C49">
         <v>86287013</v>
-      </c>
-      <c r="C49">
-        <v>108929180</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1105,10 +1105,10 @@
         <v>50</v>
       </c>
       <c r="B50">
+        <v>126743091</v>
+      </c>
+      <c r="C50">
         <v>131390270</v>
-      </c>
-      <c r="C50">
-        <v>126743091</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -1116,17 +1116,17 @@
         <v>51</v>
       </c>
       <c r="B51">
+        <v>108929184</v>
+      </c>
+      <c r="C51">
         <v>86292312</v>
-      </c>
-      <c r="C51">
-        <v>108929184</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>52</v>
       </c>
-      <c r="B52">
+      <c r="C52">
         <v>86287021</v>
       </c>
     </row>
@@ -1134,7 +1134,7 @@
       <c r="A53" t="s">
         <v>53</v>
       </c>
-      <c r="B53">
+      <c r="C53">
         <v>86287015</v>
       </c>
     </row>
@@ -1143,10 +1143,10 @@
         <v>54</v>
       </c>
       <c r="B54">
+        <v>134739034</v>
+      </c>
+      <c r="C54">
         <v>134737353</v>
-      </c>
-      <c r="C54">
-        <v>134739034</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -1154,10 +1154,10 @@
         <v>55</v>
       </c>
       <c r="B55">
+        <v>108929188</v>
+      </c>
+      <c r="C55">
         <v>86292310</v>
-      </c>
-      <c r="C55">
-        <v>108929188</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -1165,17 +1165,17 @@
         <v>56</v>
       </c>
       <c r="B56">
+        <v>1505688418</v>
+      </c>
+      <c r="C56">
         <v>1505673959</v>
-      </c>
-      <c r="C56">
-        <v>1505688418</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>57</v>
       </c>
-      <c r="B57">
+      <c r="C57">
         <v>189801181</v>
       </c>
     </row>
@@ -1183,7 +1183,7 @@
       <c r="A58" t="s">
         <v>58</v>
       </c>
-      <c r="C58">
+      <c r="B58">
         <v>108929186</v>
       </c>
     </row>
@@ -1191,7 +1191,7 @@
       <c r="A59" t="s">
         <v>59</v>
       </c>
-      <c r="C59">
+      <c r="B59">
         <v>108929182</v>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       <c r="A61" t="s">
         <v>60</v>
       </c>
-      <c r="B61">
+      <c r="C61">
         <v>126521374</v>
       </c>
     </row>
@@ -1208,10 +1208,10 @@
         <v>61</v>
       </c>
       <c r="B62">
+        <v>126740112</v>
+      </c>
+      <c r="C62">
         <v>126522961</v>
-      </c>
-      <c r="C62">
-        <v>126740112</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -1219,10 +1219,10 @@
         <v>62</v>
       </c>
       <c r="B63">
+        <v>188886689</v>
+      </c>
+      <c r="C63">
         <v>188884171</v>
-      </c>
-      <c r="C63">
-        <v>188886689</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -1230,10 +1230,10 @@
         <v>63</v>
       </c>
       <c r="B64">
+        <v>108934364</v>
+      </c>
+      <c r="C64">
         <v>86265101</v>
-      </c>
-      <c r="C64">
-        <v>108934364</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -1241,10 +1241,10 @@
         <v>64</v>
       </c>
       <c r="B65">
+        <v>134746611</v>
+      </c>
+      <c r="C65">
         <v>134730032</v>
-      </c>
-      <c r="C65">
-        <v>134746611</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -1252,10 +1252,10 @@
         <v>65</v>
       </c>
       <c r="B66">
+        <v>108934368</v>
+      </c>
+      <c r="C66">
         <v>86265105</v>
-      </c>
-      <c r="C66">
-        <v>108934368</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -1263,10 +1263,10 @@
         <v>66</v>
       </c>
       <c r="B67">
+        <v>374604904</v>
+      </c>
+      <c r="C67">
         <v>273392497</v>
-      </c>
-      <c r="C67">
-        <v>374604904</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -1274,10 +1274,10 @@
         <v>67</v>
       </c>
       <c r="B68">
+        <v>108934366</v>
+      </c>
+      <c r="C68">
         <v>86265103</v>
-      </c>
-      <c r="C68">
-        <v>108934366</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -1285,10 +1285,10 @@
         <v>68</v>
       </c>
       <c r="B69">
+        <v>108934358</v>
+      </c>
+      <c r="C69">
         <v>86264837</v>
-      </c>
-      <c r="C69">
-        <v>108934358</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -1296,17 +1296,17 @@
         <v>71</v>
       </c>
       <c r="B70">
+        <v>108934360</v>
+      </c>
+      <c r="C70">
         <v>86264839</v>
-      </c>
-      <c r="C70">
-        <v>108934360</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>69</v>
       </c>
-      <c r="B71">
+      <c r="C71">
         <v>86264847</v>
       </c>
     </row>
@@ -1315,10 +1315,10 @@
         <v>70</v>
       </c>
       <c r="B72">
+        <v>108934362</v>
+      </c>
+      <c r="C72">
         <v>86264845</v>
-      </c>
-      <c r="C72">
-        <v>108934362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>